<commit_message>
Fix: Planilha da normalizaçao
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="233">
   <si>
     <t>TABELA cancoes</t>
   </si>
@@ -311,277 +311,277 @@
     <t>usuario_id</t>
   </si>
   <si>
+    <t>idade</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>"2020-01-02 07:40:33"</t>
+  </si>
+  <si>
+    <t>Thati</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Finding My Traditions"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-05-16 06:16:22"</t>
+  </si>
+  <si>
+    <t>Cintia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Without My Love"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-10-09 12:27:48"</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Baby"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-09-21 13:14:46"</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>"2020-11-13 16:55:13"</t>
+  </si>
+  <si>
+    <t>Norman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Dance With Her Own"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-12-05 18:38:30"</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Hard And Time"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-07-30 10:00:00"</t>
+  </si>
+  <si>
+    <t>Vivian</t>
+  </si>
+  <si>
+    <t>"2021-08-15 17:10:10"</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "I Ride Alone"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2021-07-10 15:20:30"</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Honey, I'm A Lone Wolf"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2021-01-09 01:44:33"</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>"2020-07-03 19:33:28"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Rock His Everything"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-02-24 21:14:22"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-08-06 15:23:43"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Soul For Us"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-11-10 13:52:27"</t>
+  </si>
+  <si>
+    <t>TABELA usuario_planos</t>
+  </si>
+  <si>
+    <t>"2019-02-07 20:33:48"</t>
+  </si>
+  <si>
+    <t>FK - plano_id</t>
+  </si>
+  <si>
+    <t>data_assinatura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "He Heard You're Bad For Me"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-01-24 00:31:17"</t>
+  </si>
+  <si>
+    <t>2019-10-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "He Hopes We Can't Stay"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-10-12 12:35:20"</t>
+  </si>
+  <si>
+    <t>2017-12-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "Walking And Game"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2018-05-29 14:56:41"</t>
+  </si>
+  <si>
+    <t>2019-06-05</t>
+  </si>
+  <si>
+    <t>"2018-05-09 22:30:49"</t>
+  </si>
+  <si>
+    <t>2020-05-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Troubles Of My Inner Fire"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-07-27 12:52:58"</t>
+  </si>
+  <si>
+    <t>2017-02-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Celebration Of More"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2018-01-16 18:40:43"</t>
+  </si>
+  <si>
+    <t>2017-01-06</t>
+  </si>
+  <si>
+    <t>"2018-03-21 16:56:40"</t>
+  </si>
+  <si>
+    <t>2018-01-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "You Make Me Feel So.."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-10-18 13:38:05"</t>
+  </si>
+  <si>
+    <t>2018-02-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "He"s Walking Away"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2019-05-25 08:14:03"</t>
+  </si>
+  <si>
+    <t>2018-04-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "He"s Trouble"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2021-08-15 21:37:09"</t>
+  </si>
+  <si>
+    <t>2017-01-17</t>
+  </si>
+  <si>
+    <t>TABELA PLANOS</t>
+  </si>
+  <si>
+    <t>"2021-05-24 17:23:45"</t>
+  </si>
+  <si>
+    <t>plano_id</t>
+  </si>
+  <si>
+    <t>plano</t>
+  </si>
+  <si>
+    <t>preco</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Words Of Her Life"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2018-12-07 22:48:52"</t>
+  </si>
+  <si>
+    <t>gratuito</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Sweetie, Let's Go Wild"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2021-03-14 06:14:26"</t>
+  </si>
+  <si>
+    <t>familiar</t>
+  </si>
+  <si>
+    <t>7,99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "She Knows"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2020-04-01 03:36:00"</t>
+  </si>
+  <si>
+    <t>universitário</t>
+  </si>
+  <si>
+    <t>5,99</t>
+  </si>
+  <si>
+    <t>"2017-02-06 08:21:34"</t>
+  </si>
+  <si>
+    <t>pessoal</t>
+  </si>
+  <si>
+    <t>6,99</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-12-04 05:33:43"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-07-27 05:24:49"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Home Forever"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-12-25 01:03:57"</t>
+  </si>
+  <si>
     <t>usuario</t>
-  </si>
-  <si>
-    <t>idade</t>
-  </si>
-  <si>
-    <t>plano_id</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>"2020-01-02 07:40:33"</t>
-  </si>
-  <si>
-    <t>Thati</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Finding My Traditions"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-05-16 06:16:22"</t>
-  </si>
-  <si>
-    <t>Cintia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Without My Love"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-10-09 12:27:48"</t>
-  </si>
-  <si>
-    <t>Bill</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Baby"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-09-21 13:14:46"</t>
-  </si>
-  <si>
-    <t>Roger</t>
-  </si>
-  <si>
-    <t>"2020-11-13 16:55:13"</t>
-  </si>
-  <si>
-    <t>Norman</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Dance With Her Own"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-12-05 18:38:30"</t>
-  </si>
-  <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Hard And Time"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-07-30 10:00:00"</t>
-  </si>
-  <si>
-    <t>Vivian</t>
-  </si>
-  <si>
-    <t>"2021-08-15 17:10:10"</t>
-  </si>
-  <si>
-    <t>Carol</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "I Ride Alone"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2021-07-10 15:20:30"</t>
-  </si>
-  <si>
-    <t>Angelina</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Honey, I'm A Lone Wolf"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2021-01-09 01:44:33"</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>"2020-07-03 19:33:28"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Rock His Everything"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-02-24 21:14:22"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-08-06 15:23:43"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Soul For Us"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-11-10 13:52:27"</t>
-  </si>
-  <si>
-    <t>TABELA usuario_planos</t>
-  </si>
-  <si>
-    <t>"2019-02-07 20:33:48"</t>
-  </si>
-  <si>
-    <t>FK - plano_id</t>
-  </si>
-  <si>
-    <t>data_assinatura</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "He Heard You're Bad For Me"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-01-24 00:31:17"</t>
-  </si>
-  <si>
-    <t>2019-10-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "He Hopes We Can't Stay"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-10-12 12:35:20"</t>
-  </si>
-  <si>
-    <t>2017-12-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Walking And Game"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2018-05-29 14:56:41"</t>
-  </si>
-  <si>
-    <t>2019-06-05</t>
-  </si>
-  <si>
-    <t>"2018-05-09 22:30:49"</t>
-  </si>
-  <si>
-    <t>2020-05-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Troubles Of My Inner Fire"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-07-27 12:52:58"</t>
-  </si>
-  <si>
-    <t>2017-02-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Celebration Of More"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2018-01-16 18:40:43"</t>
-  </si>
-  <si>
-    <t>2017-01-06</t>
-  </si>
-  <si>
-    <t>"2018-03-21 16:56:40"</t>
-  </si>
-  <si>
-    <t>2018-01-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "You Make Me Feel So.."</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-10-18 13:38:05"</t>
-  </si>
-  <si>
-    <t>2018-02-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "He"s Walking Away"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2019-05-25 08:14:03"</t>
-  </si>
-  <si>
-    <t>2018-04-29</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "He"s Trouble"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2021-08-15 21:37:09"</t>
-  </si>
-  <si>
-    <t>2017-01-17</t>
-  </si>
-  <si>
-    <t>TABELA PLANOS</t>
-  </si>
-  <si>
-    <t>"2021-05-24 17:23:45"</t>
-  </si>
-  <si>
-    <t>plano</t>
-  </si>
-  <si>
-    <t>preco</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Words Of Her Life"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2018-12-07 22:48:52"</t>
-  </si>
-  <si>
-    <t>gratuito</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Sweetie, Let's Go Wild"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2021-03-14 06:14:26"</t>
-  </si>
-  <si>
-    <t>familiar</t>
-  </si>
-  <si>
-    <t>7,99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "She Knows"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-04-01 03:36:00"</t>
-  </si>
-  <si>
-    <t>universitário</t>
-  </si>
-  <si>
-    <t>5,99</t>
-  </si>
-  <si>
-    <t>"2017-02-06 08:21:34"</t>
-  </si>
-  <si>
-    <t>pessoal</t>
-  </si>
-  <si>
-    <t>6,99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-12-04 05:33:43"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-07-27 05:24:49"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Home Forever"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-12-25 01:03:57"</t>
   </si>
   <si>
     <t>valor_plano</t>
@@ -2982,18 +2982,15 @@
       <c r="E53" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="F53" s="50" t="s">
+      <c r="F53" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="50" t="s">
         <v>99</v>
-      </c>
-      <c r="G53" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="H53" s="40" t="s">
-        <v>101</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K53" s="12">
         <v>5.0</v>
@@ -3016,23 +3013,20 @@
         <v>65</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E54" s="51">
         <v>1.0</v>
       </c>
       <c r="F54" s="51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G54" s="51">
         <v>23.0</v>
       </c>
-      <c r="H54" s="40">
-        <v>1.0</v>
-      </c>
       <c r="I54" s="10"/>
       <c r="J54" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K54" s="12">
         <v>6.0</v>
@@ -3052,22 +3046,19 @@
         <v>2.0</v>
       </c>
       <c r="B55" s="51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C55" s="51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E55" s="51">
         <v>2.0</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G55" s="51">
         <v>35.0</v>
-      </c>
-      <c r="H55" s="40">
-        <v>2.0</v>
       </c>
       <c r="I55" s="10"/>
       <c r="J55" s="25">
@@ -3091,22 +3082,19 @@
         <v>2.0</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C56" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E56" s="51">
         <v>3.0</v>
       </c>
       <c r="F56" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G56" s="51">
         <v>20.0</v>
-      </c>
-      <c r="H56" s="40">
-        <v>3.0</v>
       </c>
       <c r="I56" s="10"/>
       <c r="J56" s="25">
@@ -3130,22 +3118,19 @@
         <v>2.0</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C57" s="51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E57" s="51">
         <v>4.0</v>
       </c>
       <c r="F57" s="51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G57" s="51">
         <v>45.0</v>
-      </c>
-      <c r="H57" s="40">
-        <v>4.0</v>
       </c>
       <c r="I57" s="53"/>
       <c r="J57" s="25">
@@ -3173,19 +3158,16 @@
         <v>12</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E58" s="51">
         <v>5.0</v>
       </c>
       <c r="F58" s="51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G58" s="51">
         <v>58.0</v>
-      </c>
-      <c r="H58" s="40">
-        <v>4.0</v>
       </c>
       <c r="I58" s="10"/>
       <c r="J58" s="54">
@@ -3210,22 +3192,19 @@
         <v>3.0</v>
       </c>
       <c r="B59" s="51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" s="51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E59" s="51">
         <v>6.0</v>
       </c>
       <c r="F59" s="51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G59" s="51">
         <v>33.0</v>
-      </c>
-      <c r="H59" s="40">
-        <v>2.0</v>
       </c>
       <c r="I59" s="10"/>
       <c r="J59" s="54">
@@ -3249,22 +3228,19 @@
         <v>3.0</v>
       </c>
       <c r="B60" s="51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" s="51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E60" s="51">
         <v>7.0</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G60" s="51">
         <v>26.0</v>
-      </c>
-      <c r="H60" s="40">
-        <v>3.0</v>
       </c>
       <c r="I60" s="10"/>
       <c r="J60" s="54">
@@ -3292,19 +3268,16 @@
         <v>8</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E61" s="51">
         <v>8.0</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G61" s="51">
         <v>19.0</v>
-      </c>
-      <c r="H61" s="40">
-        <v>3.0</v>
       </c>
       <c r="I61" s="4"/>
       <c r="J61" s="54">
@@ -3329,22 +3302,19 @@
         <v>4.0</v>
       </c>
       <c r="B62" s="51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C62" s="51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E62" s="51">
         <v>9.0</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G62" s="51">
         <v>42.0</v>
-      </c>
-      <c r="H62" s="40">
-        <v>2.0</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="56">
@@ -3369,22 +3339,19 @@
         <v>4.0</v>
       </c>
       <c r="B63" s="51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C63" s="51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E63" s="51">
         <v>10.0</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G63" s="51">
         <v>46.0</v>
-      </c>
-      <c r="H63" s="40">
-        <v>2.0</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="56">
@@ -3412,7 +3379,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="30"/>
@@ -3441,10 +3408,10 @@
         <v>5.0</v>
       </c>
       <c r="B65" s="51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="48"/>
@@ -3476,7 +3443,7 @@
         <v>93</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="48"/>
@@ -3505,13 +3472,13 @@
         <v>5.0</v>
       </c>
       <c r="B67" s="51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="E67" s="41" t="s">
         <v>134</v>
-      </c>
-      <c r="C67" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="E67" s="41" t="s">
-        <v>136</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="3"/>
@@ -3534,16 +3501,16 @@
         <v>69</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E68" s="49" t="s">
         <v>74</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G68" s="50" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L68" s="26"/>
       <c r="M68" s="26"/>
@@ -3561,10 +3528,10 @@
         <v>6.0</v>
       </c>
       <c r="B69" s="51" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C69" s="51" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E69" s="51">
         <v>1.0</v>
@@ -3573,7 +3540,7 @@
         <v>1.0</v>
       </c>
       <c r="G69" s="51" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L69" s="26"/>
       <c r="M69" s="26"/>
@@ -3592,10 +3559,10 @@
         <v>6.0</v>
       </c>
       <c r="B70" s="51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C70" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D70" s="26"/>
       <c r="E70" s="51">
@@ -3605,7 +3572,7 @@
         <v>2.0</v>
       </c>
       <c r="G70" s="51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L70" s="26"/>
       <c r="M70" s="26"/>
@@ -3624,10 +3591,10 @@
         <v>6.0</v>
       </c>
       <c r="B71" s="51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C71" s="51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E71" s="51">
         <v>3.0</v>
@@ -3636,7 +3603,7 @@
         <v>3.0</v>
       </c>
       <c r="G71" s="51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L71" s="26"/>
       <c r="M71" s="26"/>
@@ -3658,7 +3625,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E72" s="51">
         <v>4.0</v>
@@ -3667,7 +3634,7 @@
         <v>4.0</v>
       </c>
       <c r="G72" s="51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
@@ -3684,10 +3651,10 @@
         <v>7.0</v>
       </c>
       <c r="B73" s="51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C73" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E73" s="51">
         <v>5.0</v>
@@ -3696,7 +3663,7 @@
         <v>4.0</v>
       </c>
       <c r="G73" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
@@ -3713,10 +3680,10 @@
         <v>7.0</v>
       </c>
       <c r="B74" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C74" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E74" s="51">
         <v>6.0</v>
@@ -3725,7 +3692,7 @@
         <v>2.0</v>
       </c>
       <c r="G74" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -3748,7 +3715,7 @@
         <v>70</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E75" s="51">
         <v>7.0</v>
@@ -3757,7 +3724,7 @@
         <v>3.0</v>
       </c>
       <c r="G75" s="51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
@@ -3777,10 +3744,10 @@
         <v>8.0</v>
       </c>
       <c r="B76" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C76" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E76" s="51">
         <v>8.0</v>
@@ -3789,7 +3756,7 @@
         <v>3.0</v>
       </c>
       <c r="G76" s="51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -3809,10 +3776,10 @@
         <v>8.0</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C77" s="51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E77" s="51">
         <v>9.0</v>
@@ -3821,7 +3788,7 @@
         <v>2.0</v>
       </c>
       <c r="G77" s="51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
@@ -3842,10 +3809,10 @@
         <v>8.0</v>
       </c>
       <c r="B78" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C78" s="51" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E78" s="51">
         <v>10.0</v>
@@ -3854,11 +3821,11 @@
         <v>2.0</v>
       </c>
       <c r="G78" s="51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H78" s="30"/>
       <c r="I78" s="36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="M78" s="4"/>
       <c r="N78" s="10"/>
@@ -3879,20 +3846,20 @@
         <v>22</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="7" t="s">
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="J79" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K79" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="K79" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="M79" s="4"/>
       <c r="N79" s="10"/>
@@ -3910,16 +3877,16 @@
         <v>9.0</v>
       </c>
       <c r="B80" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" s="51" t="s">
         <v>172</v>
-      </c>
-      <c r="C80" s="51" t="s">
-        <v>173</v>
       </c>
       <c r="I80" s="16">
         <v>1.0</v>
       </c>
       <c r="J80" s="58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K80" s="59">
         <v>0.0</v>
@@ -3940,19 +3907,19 @@
         <v>9.0</v>
       </c>
       <c r="B81" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="51" t="s">
         <v>175</v>
-      </c>
-      <c r="C81" s="51" t="s">
-        <v>176</v>
       </c>
       <c r="I81" s="16">
         <v>2.0</v>
       </c>
       <c r="J81" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="K81" s="59" t="s">
         <v>177</v>
-      </c>
-      <c r="K81" s="59" t="s">
-        <v>178</v>
       </c>
       <c r="M81" s="4"/>
       <c r="N81" s="10"/>
@@ -3970,19 +3937,19 @@
         <v>9.0</v>
       </c>
       <c r="B82" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C82" s="51" t="s">
         <v>179</v>
-      </c>
-      <c r="C82" s="51" t="s">
-        <v>180</v>
       </c>
       <c r="I82" s="16">
         <v>3.0</v>
       </c>
       <c r="J82" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="K82" s="59" t="s">
         <v>181</v>
-      </c>
-      <c r="K82" s="59" t="s">
-        <v>182</v>
       </c>
       <c r="M82" s="4"/>
       <c r="N82" s="10"/>
@@ -4003,16 +3970,16 @@
         <v>26</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I83" s="16">
         <v>4.0</v>
       </c>
       <c r="J83" s="58" t="s">
+        <v>183</v>
+      </c>
+      <c r="K83" s="59" t="s">
         <v>184</v>
-      </c>
-      <c r="K83" s="59" t="s">
-        <v>185</v>
       </c>
       <c r="M83" s="4"/>
       <c r="N83" s="10"/>
@@ -4030,10 +3997,10 @@
         <v>10.0</v>
       </c>
       <c r="B84" s="51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C84" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M84" s="4"/>
       <c r="N84" s="10"/>
@@ -4051,10 +4018,10 @@
         <v>10.0</v>
       </c>
       <c r="B85" s="51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C85" s="51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M85" s="4"/>
       <c r="N85" s="10"/>
@@ -4072,10 +4039,10 @@
         <v>10.0</v>
       </c>
       <c r="B86" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" s="51" t="s">
         <v>188</v>
-      </c>
-      <c r="C86" s="51" t="s">
-        <v>189</v>
       </c>
       <c r="M86" s="4"/>
       <c r="N86" s="10"/>
@@ -7163,10 +7130,10 @@
         <v>98</v>
       </c>
       <c r="B1" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="60" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>100</v>
       </c>
       <c r="D1" s="60" t="s">
         <v>81</v>
@@ -7175,10 +7142,10 @@
         <v>82</v>
       </c>
       <c r="F1" s="60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H1" s="60" t="s">
         <v>190</v>
@@ -7189,7 +7156,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="60">
         <v>23.0</v>
@@ -7201,10 +7168,10 @@
         <v>192</v>
       </c>
       <c r="F2" s="60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="60" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H2" s="60">
         <v>0.0</v>
@@ -7215,7 +7182,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="60">
         <v>35.0</v>
@@ -7227,13 +7194,13 @@
         <v>194</v>
       </c>
       <c r="F3" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="60" t="s">
         <v>177</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="H3" s="60" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4">
@@ -7241,7 +7208,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="60">
         <v>20.0</v>
@@ -7253,13 +7220,13 @@
         <v>196</v>
       </c>
       <c r="F4" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="60" t="s">
         <v>181</v>
-      </c>
-      <c r="G4" s="60" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" s="60" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5">
@@ -7267,7 +7234,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="60">
         <v>45.0</v>
@@ -7279,13 +7246,13 @@
         <v>198</v>
       </c>
       <c r="F5" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" s="60" t="s">
         <v>184</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>150</v>
-      </c>
-      <c r="H5" s="60" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="6">
@@ -7293,7 +7260,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="60">
         <v>58.0</v>
@@ -7305,13 +7272,13 @@
         <v>200</v>
       </c>
       <c r="F6" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="60" t="s">
         <v>184</v>
-      </c>
-      <c r="G6" s="60" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" s="60" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7">
@@ -7319,7 +7286,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="60">
         <v>33.0</v>
@@ -7331,13 +7298,13 @@
         <v>202</v>
       </c>
       <c r="F7" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="60" t="s">
         <v>177</v>
-      </c>
-      <c r="G7" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="60" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="8">
@@ -7345,7 +7312,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="60">
         <v>26.0</v>
@@ -7357,13 +7324,13 @@
         <v>204</v>
       </c>
       <c r="F8" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="60" t="s">
         <v>181</v>
-      </c>
-      <c r="G8" s="60" t="s">
-        <v>158</v>
-      </c>
-      <c r="H8" s="60" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="9">
@@ -7371,7 +7338,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" s="60">
         <v>19.0</v>
@@ -7383,13 +7350,13 @@
         <v>206</v>
       </c>
       <c r="F9" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="60" t="s">
         <v>181</v>
-      </c>
-      <c r="G9" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="H9" s="60" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10">
@@ -7397,7 +7364,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" s="60">
         <v>42.0</v>
@@ -7409,13 +7376,13 @@
         <v>208</v>
       </c>
       <c r="F10" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" s="60" t="s">
         <v>177</v>
-      </c>
-      <c r="G10" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="H10" s="60" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="11">
@@ -7423,7 +7390,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="60">
         <v>46.0</v>
@@ -7435,13 +7402,13 @@
         <v>210</v>
       </c>
       <c r="F11" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="60" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="60" t="s">
         <v>177</v>
-      </c>
-      <c r="G11" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="H11" s="60" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
Fix: Planilha da normalizaçao TABELA historico_usuario
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="208">
   <si>
     <t>TABELA cancoes</t>
   </si>
@@ -275,9 +275,6 @@
     <t>Tyler Isle</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Walking And Man"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-05-02 05:30:35"</t>
   </si>
   <si>
@@ -287,24 +284,15 @@
     <t>Fog</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Young And Father"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-03-06 11:22:33"</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Diamond Power"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-08-05 08:05:17"</t>
   </si>
   <si>
     <t>TABELA usuario</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Let's Be Silly"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-09-14 16:32:22"</t>
   </si>
   <si>
@@ -323,27 +311,18 @@
     <t>Thati</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Finding My Traditions"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-05-16 06:16:22"</t>
   </si>
   <si>
     <t>Cintia</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Without My Love"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-10-09 12:27:48"</t>
   </si>
   <si>
     <t>Bill</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Baby"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-09-21 13:14:46"</t>
   </si>
   <si>
@@ -356,18 +335,12 @@
     <t>Norman</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Dance With Her Own"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-12-05 18:38:30"</t>
   </si>
   <si>
     <t>Patrick</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Hard And Time"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-07-30 10:00:00"</t>
   </si>
   <si>
@@ -380,18 +353,12 @@
     <t>Carol</t>
   </si>
   <si>
-    <t xml:space="preserve"> "I Ride Alone"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2021-07-10 15:20:30"</t>
   </si>
   <si>
     <t>Angelina</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Honey, I'm A Lone Wolf"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2021-01-09 01:44:33"</t>
   </si>
   <si>
@@ -401,18 +368,12 @@
     <t>"2020-07-03 19:33:28"</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Rock His Everything"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2017-02-24 21:14:22"</t>
   </si>
   <si>
     <t xml:space="preserve"> "2020-08-06 15:23:43"</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Soul For Us"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-11-10 13:52:27"</t>
   </si>
   <si>
@@ -428,27 +389,18 @@
     <t>data_assinatura</t>
   </si>
   <si>
-    <t xml:space="preserve"> "He Heard You're Bad For Me"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2017-01-24 00:31:17"</t>
   </si>
   <si>
     <t>2019-10-20</t>
   </si>
   <si>
-    <t xml:space="preserve"> "He Hopes We Can't Stay"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2017-10-12 12:35:20"</t>
   </si>
   <si>
     <t>2017-12-30</t>
   </si>
   <si>
-    <t xml:space="preserve">  "Walking And Game"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2018-05-29 14:56:41"</t>
   </si>
   <si>
@@ -461,18 +413,12 @@
     <t>2020-05-13</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Troubles Of My Inner Fire"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-07-27 12:52:58"</t>
   </si>
   <si>
     <t>2017-02-17</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Celebration Of More"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2018-01-16 18:40:43"</t>
   </si>
   <si>
@@ -485,27 +431,18 @@
     <t>2018-01-05</t>
   </si>
   <si>
-    <t xml:space="preserve"> "You Make Me Feel So.."</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2020-10-18 13:38:05"</t>
   </si>
   <si>
     <t>2018-02-14</t>
   </si>
   <si>
-    <t xml:space="preserve"> "He"s Walking Away"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2019-05-25 08:14:03"</t>
   </si>
   <si>
     <t>2018-04-29</t>
   </si>
   <si>
-    <t xml:space="preserve"> "He"s Trouble"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2021-08-15 21:37:09"</t>
   </si>
   <si>
@@ -527,88 +464,76 @@
     <t>preco</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Words Of Her Life"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2018-12-07 22:48:52"</t>
   </si>
   <si>
     <t>gratuito</t>
   </si>
   <si>
-    <t xml:space="preserve"> "Sweetie, Let's Go Wild"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "2021-03-14 06:14:26"</t>
   </si>
   <si>
     <t>familiar</t>
   </si>
   <si>
+    <t xml:space="preserve"> "2020-04-01 03:36:00"</t>
+  </si>
+  <si>
+    <t>universitário</t>
+  </si>
+  <si>
+    <t>"2017-02-06 08:21:34"</t>
+  </si>
+  <si>
+    <t>pessoal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-12-04 05:33:43"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-07-27 05:24:49"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "2017-12-25 01:03:57"</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>valor_plano</t>
+  </si>
+  <si>
+    <t>Honey"; "Walking And Man"; "Young And Father"; "Diamond Power"; "Let's Be Silly"</t>
+  </si>
+  <si>
+    <t>2020-02-28 10:45:55"; "2020-05-02 05:30:35"; "2020-03-06 11:22:33"; "2020-08-05 08:05:17"; "2020-09-14 16:32:22"</t>
+  </si>
+  <si>
+    <t>I Heard I Want To Bo Alone"; "Finding My Traditions"; "Without My Love"; "Baby"</t>
+  </si>
+  <si>
+    <t>2020-01-02 07:40:33"; "2020-05-16 06:16:22"; "2020-10-09 12:27:48"; "2020-09-21 13:14:46"</t>
+  </si>
+  <si>
     <t>7,99</t>
   </si>
   <si>
-    <t xml:space="preserve"> "She Knows"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2020-04-01 03:36:00"</t>
-  </si>
-  <si>
-    <t>universitário</t>
+    <t>Magic Circus"; "Dance With Her Own"; "Hard And Time"</t>
+  </si>
+  <si>
+    <t>2020-11-13 16:55:13"; "2020-12-05 18:38:30"; "2020-07-30 10:00:00"</t>
   </si>
   <si>
     <t>5,99</t>
   </si>
   <si>
-    <t>"2017-02-06 08:21:34"</t>
-  </si>
-  <si>
-    <t>pessoal</t>
+    <t>Reflections Of Magic"; "I Ride Alone"; "Honey, I'm A Lone Wolf"</t>
+  </si>
+  <si>
+    <t>2021-08-15 17:10:10"; "2021-07-10 15:20:30"; "2021-01-09 01:44:33"</t>
   </si>
   <si>
     <t>6,99</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-12-04 05:33:43"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-07-27 05:24:49"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "Home Forever"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "2017-12-25 01:03:57"</t>
-  </si>
-  <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>valor_plano</t>
-  </si>
-  <si>
-    <t>Honey"; "Walking And Man"; "Young And Father"; "Diamond Power"; "Let's Be Silly"</t>
-  </si>
-  <si>
-    <t>2020-02-28 10:45:55"; "2020-05-02 05:30:35"; "2020-03-06 11:22:33"; "2020-08-05 08:05:17"; "2020-09-14 16:32:22"</t>
-  </si>
-  <si>
-    <t>I Heard I Want To Bo Alone"; "Finding My Traditions"; "Without My Love"; "Baby"</t>
-  </si>
-  <si>
-    <t>2020-01-02 07:40:33"; "2020-05-16 06:16:22"; "2020-10-09 12:27:48"; "2020-09-21 13:14:46"</t>
-  </si>
-  <si>
-    <t>Magic Circus"; "Dance With Her Own"; "Hard And Time"</t>
-  </si>
-  <si>
-    <t>2020-11-13 16:55:13"; "2020-12-05 18:38:30"; "2020-07-30 10:00:00"</t>
-  </si>
-  <si>
-    <t>Reflections Of Magic"; "I Ride Alone"; "Honey, I'm A Lone Wolf"</t>
-  </si>
-  <si>
-    <t>2021-08-15 17:10:10"; "2021-07-10 15:20:30"; "2021-01-09 01:44:33"</t>
   </si>
   <si>
     <t>Honey, So Do I"; "Rock His Everything"; "Diamond Power"; "Soul For Us"</t>
@@ -742,7 +667,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,6 +690,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -842,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -980,6 +911,15 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -990,11 +930,23 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1304,9 +1256,9 @@
     <col customWidth="1" min="3" max="3" width="21.29"/>
     <col customWidth="1" min="4" max="4" width="28.43"/>
     <col customWidth="1" min="5" max="5" width="21.14"/>
-    <col customWidth="1" min="6" max="6" width="15.43"/>
+    <col customWidth="1" min="6" max="6" width="13.29"/>
     <col customWidth="1" min="7" max="7" width="14.71"/>
-    <col customWidth="1" min="8" max="8" width="17.0"/>
+    <col customWidth="1" min="8" max="8" width="13.29"/>
     <col customWidth="1" min="9" max="9" width="20.86"/>
     <col customWidth="1" min="10" max="10" width="26.71"/>
     <col customWidth="1" min="11" max="11" width="17.71"/>
@@ -2851,8 +2803,8 @@
       <c r="A49" s="51">
         <v>1.0</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>67</v>
+      <c r="B49" s="16">
+        <v>36.0</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>85</v>
@@ -2882,15 +2834,15 @@
       <c r="A50" s="51">
         <v>1.0</v>
       </c>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="16">
+        <v>25.0</v>
+      </c>
+      <c r="C50" s="51" t="s">
         <v>87</v>
-      </c>
-      <c r="C50" s="51" t="s">
-        <v>88</v>
       </c>
       <c r="G50" s="30"/>
       <c r="J50" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K50" s="12">
         <v>4.0</v>
@@ -2900,7 +2852,7 @@
         <v>6.0</v>
       </c>
       <c r="N50" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q50" s="10"/>
       <c r="R50" s="4"/>
@@ -2913,16 +2865,16 @@
       <c r="A51" s="51">
         <v>1.0</v>
       </c>
-      <c r="B51" s="51" t="s">
-        <v>91</v>
+      <c r="B51" s="16">
+        <v>23.0</v>
       </c>
       <c r="C51" s="51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E51" s="26"/>
       <c r="G51" s="30"/>
       <c r="J51" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K51" s="12">
         <v>1.0</v>
@@ -2940,14 +2892,14 @@
       <c r="A52" s="51">
         <v>1.0</v>
       </c>
-      <c r="B52" s="51" t="s">
-        <v>93</v>
+      <c r="B52" s="16">
+        <v>14.0</v>
       </c>
       <c r="C52" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="E52" s="53" t="s">
+        <v>92</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="3"/>
@@ -2972,25 +2924,25 @@
       <c r="A53" s="51">
         <v>1.0</v>
       </c>
-      <c r="B53" s="51" t="s">
-        <v>96</v>
+      <c r="B53" s="16">
+        <v>15.0</v>
       </c>
       <c r="C53" s="51" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D53" s="30"/>
-      <c r="E53" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" s="49" t="s">
+      <c r="E53" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="G53" s="50" t="s">
-        <v>99</v>
+      <c r="G53" s="54" t="s">
+        <v>95</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K53" s="12">
         <v>5.0</v>
@@ -3009,24 +2961,24 @@
       <c r="A54" s="51">
         <v>2.0</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>65</v>
+      <c r="B54" s="16">
+        <v>34.0</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E54" s="51">
         <v>1.0</v>
       </c>
       <c r="F54" s="51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G54" s="51">
         <v>23.0</v>
       </c>
       <c r="I54" s="10"/>
       <c r="J54" s="25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K54" s="12">
         <v>6.0</v>
@@ -3045,17 +2997,17 @@
       <c r="A55" s="51">
         <v>2.0</v>
       </c>
-      <c r="B55" s="51" t="s">
-        <v>103</v>
+      <c r="B55" s="16">
+        <v>24.0</v>
       </c>
       <c r="C55" s="51" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E55" s="51">
         <v>2.0</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G55" s="51">
         <v>35.0</v>
@@ -3081,17 +3033,17 @@
       <c r="A56" s="51">
         <v>2.0</v>
       </c>
-      <c r="B56" s="51" t="s">
-        <v>106</v>
+      <c r="B56" s="16">
+        <v>21.0</v>
       </c>
       <c r="C56" s="51" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E56" s="51">
         <v>3.0</v>
       </c>
       <c r="F56" s="51" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G56" s="51">
         <v>20.0</v>
@@ -3117,22 +3069,22 @@
       <c r="A57" s="51">
         <v>2.0</v>
       </c>
-      <c r="B57" s="51" t="s">
-        <v>109</v>
+      <c r="B57" s="16">
+        <v>39.0</v>
       </c>
       <c r="C57" s="51" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E57" s="51">
         <v>4.0</v>
       </c>
       <c r="F57" s="51" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G57" s="51">
         <v>45.0</v>
       </c>
-      <c r="I57" s="53"/>
+      <c r="I57" s="56"/>
       <c r="J57" s="25">
         <v>6.0</v>
       </c>
@@ -3154,26 +3106,26 @@
       <c r="A58" s="51">
         <v>3.0</v>
       </c>
-      <c r="B58" s="16" t="s">
-        <v>12</v>
+      <c r="B58" s="16">
+        <v>6.0</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E58" s="51">
         <v>5.0</v>
       </c>
       <c r="F58" s="51" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G58" s="51">
         <v>58.0</v>
       </c>
       <c r="I58" s="10"/>
-      <c r="J58" s="54">
+      <c r="J58" s="57">
         <v>7.0</v>
       </c>
-      <c r="K58" s="55">
+      <c r="K58" s="58">
         <v>4.0</v>
       </c>
       <c r="L58" s="26"/>
@@ -3191,26 +3143,26 @@
       <c r="A59" s="51">
         <v>3.0</v>
       </c>
-      <c r="B59" s="51" t="s">
-        <v>114</v>
+      <c r="B59" s="16">
+        <v>3.0</v>
       </c>
       <c r="C59" s="51" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E59" s="51">
         <v>6.0</v>
       </c>
       <c r="F59" s="51" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G59" s="51">
         <v>33.0</v>
       </c>
       <c r="I59" s="10"/>
-      <c r="J59" s="54">
+      <c r="J59" s="57">
         <v>7.0</v>
       </c>
-      <c r="K59" s="55">
+      <c r="K59" s="58">
         <v>5.0</v>
       </c>
       <c r="L59" s="26"/>
@@ -3227,26 +3179,26 @@
       <c r="A60" s="51">
         <v>3.0</v>
       </c>
-      <c r="B60" s="51" t="s">
-        <v>117</v>
+      <c r="B60" s="16">
+        <v>26.0</v>
       </c>
       <c r="C60" s="51" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E60" s="51">
         <v>7.0</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G60" s="51">
         <v>26.0</v>
       </c>
       <c r="I60" s="10"/>
-      <c r="J60" s="54">
+      <c r="J60" s="57">
         <v>8.0</v>
       </c>
-      <c r="K60" s="55">
+      <c r="K60" s="58">
         <v>1.0</v>
       </c>
       <c r="L60" s="26"/>
@@ -3264,26 +3216,26 @@
       <c r="A61" s="51">
         <v>4.0</v>
       </c>
-      <c r="B61" s="16" t="s">
-        <v>8</v>
+      <c r="B61" s="16">
+        <v>2.0</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E61" s="51">
         <v>8.0</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G61" s="51">
         <v>19.0</v>
       </c>
       <c r="I61" s="4"/>
-      <c r="J61" s="54">
+      <c r="J61" s="57">
         <v>8.0</v>
       </c>
-      <c r="K61" s="55">
+      <c r="K61" s="58">
         <v>5.0</v>
       </c>
       <c r="L61" s="26"/>
@@ -3301,23 +3253,23 @@
       <c r="A62" s="51">
         <v>4.0</v>
       </c>
-      <c r="B62" s="51" t="s">
-        <v>122</v>
+      <c r="B62" s="16">
+        <v>35.0</v>
       </c>
       <c r="C62" s="51" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E62" s="51">
         <v>9.0</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G62" s="51">
         <v>42.0</v>
       </c>
       <c r="I62" s="4"/>
-      <c r="J62" s="56">
+      <c r="J62" s="59">
         <v>9.0</v>
       </c>
       <c r="K62" s="16">
@@ -3338,23 +3290,23 @@
       <c r="A63" s="51">
         <v>4.0</v>
       </c>
-      <c r="B63" s="51" t="s">
-        <v>125</v>
+      <c r="B63" s="16">
+        <v>27.0</v>
       </c>
       <c r="C63" s="51" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E63" s="51">
         <v>10.0</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G63" s="51">
         <v>46.0</v>
       </c>
       <c r="I63" s="4"/>
-      <c r="J63" s="56">
+      <c r="J63" s="59">
         <v>9.0</v>
       </c>
       <c r="K63" s="16">
@@ -3375,17 +3327,17 @@
       <c r="A64" s="51">
         <v>5.0</v>
       </c>
-      <c r="B64" s="16" t="s">
-        <v>13</v>
+      <c r="B64" s="16">
+        <v>7.0</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="30"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="56">
+      <c r="J64" s="59">
         <v>9.0</v>
       </c>
       <c r="K64" s="16">
@@ -3407,17 +3359,17 @@
       <c r="A65" s="51">
         <v>5.0</v>
       </c>
-      <c r="B65" s="51" t="s">
-        <v>129</v>
+      <c r="B65" s="16">
+        <v>12.0</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="48"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="56">
+      <c r="J65" s="59">
         <v>10.0</v>
       </c>
       <c r="K65" s="16">
@@ -3439,17 +3391,17 @@
       <c r="A66" s="51">
         <v>5.0</v>
       </c>
-      <c r="B66" s="51" t="s">
-        <v>93</v>
+      <c r="B66" s="16">
+        <v>14.0</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="48"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="56">
+      <c r="J66" s="59">
         <v>10.0</v>
       </c>
       <c r="K66" s="16">
@@ -3471,14 +3423,14 @@
       <c r="A67" s="51">
         <v>5.0</v>
       </c>
-      <c r="B67" s="51" t="s">
-        <v>132</v>
+      <c r="B67" s="16">
+        <v>1.0</v>
       </c>
       <c r="C67" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="E67" s="41" t="s">
-        <v>134</v>
+        <v>120</v>
+      </c>
+      <c r="E67" s="60" t="s">
+        <v>121</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="3"/>
@@ -3497,26 +3449,26 @@
       <c r="A68" s="51">
         <v>6.0</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>69</v>
+      <c r="B68" s="16">
+        <v>38.0</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E68" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="F68" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="G68" s="50" t="s">
-        <v>137</v>
+      <c r="F68" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="G68" s="54" t="s">
+        <v>124</v>
       </c>
       <c r="L68" s="26"/>
       <c r="M68" s="26"/>
       <c r="N68" s="10"/>
       <c r="O68" s="10"/>
-      <c r="P68" s="57"/>
+      <c r="P68" s="61"/>
       <c r="R68" s="4"/>
       <c r="S68" s="4"/>
       <c r="T68" s="4"/>
@@ -3527,11 +3479,11 @@
       <c r="A69" s="51">
         <v>6.0</v>
       </c>
-      <c r="B69" s="51" t="s">
-        <v>138</v>
+      <c r="B69" s="16">
+        <v>29.0</v>
       </c>
       <c r="C69" s="51" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E69" s="51">
         <v>1.0</v>
@@ -3540,7 +3492,7 @@
         <v>1.0</v>
       </c>
       <c r="G69" s="51" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="L69" s="26"/>
       <c r="M69" s="26"/>
@@ -3558,11 +3510,11 @@
       <c r="A70" s="51">
         <v>6.0</v>
       </c>
-      <c r="B70" s="51" t="s">
-        <v>141</v>
+      <c r="B70" s="16">
+        <v>30.0</v>
       </c>
       <c r="C70" s="51" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D70" s="26"/>
       <c r="E70" s="51">
@@ -3572,7 +3524,7 @@
         <v>2.0</v>
       </c>
       <c r="G70" s="51" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="L70" s="26"/>
       <c r="M70" s="26"/>
@@ -3590,11 +3542,11 @@
       <c r="A71" s="51">
         <v>6.0</v>
       </c>
-      <c r="B71" s="51" t="s">
-        <v>144</v>
+      <c r="B71" s="16">
+        <v>22.0</v>
       </c>
       <c r="C71" s="51" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="E71" s="51">
         <v>3.0</v>
@@ -3603,7 +3555,7 @@
         <v>3.0</v>
       </c>
       <c r="G71" s="51" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="L71" s="26"/>
       <c r="M71" s="26"/>
@@ -3621,11 +3573,11 @@
       <c r="A72" s="51">
         <v>7.0</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>11</v>
+      <c r="B72" s="16">
+        <v>5.0</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="E72" s="51">
         <v>4.0</v>
@@ -3634,7 +3586,7 @@
         <v>4.0</v>
       </c>
       <c r="G72" s="51" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
@@ -3650,11 +3602,11 @@
       <c r="A73" s="51">
         <v>7.0</v>
       </c>
-      <c r="B73" s="51" t="s">
-        <v>149</v>
+      <c r="B73" s="16">
+        <v>4.0</v>
       </c>
       <c r="C73" s="51" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="E73" s="51">
         <v>5.0</v>
@@ -3663,7 +3615,7 @@
         <v>4.0</v>
       </c>
       <c r="G73" s="51" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
@@ -3679,11 +3631,11 @@
       <c r="A74" s="51">
         <v>7.0</v>
       </c>
-      <c r="B74" s="51" t="s">
-        <v>152</v>
+      <c r="B74" s="16">
+        <v>11.0</v>
       </c>
       <c r="C74" s="51" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="E74" s="51">
         <v>6.0</v>
@@ -3692,7 +3644,7 @@
         <v>2.0</v>
       </c>
       <c r="G74" s="51" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
@@ -3711,11 +3663,11 @@
       <c r="A75" s="51">
         <v>8.0</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>70</v>
+      <c r="B75" s="16">
+        <v>39.0</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="E75" s="51">
         <v>7.0</v>
@@ -3724,7 +3676,7 @@
         <v>3.0</v>
       </c>
       <c r="G75" s="51" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
@@ -3743,11 +3695,11 @@
       <c r="A76" s="51">
         <v>8.0</v>
       </c>
-      <c r="B76" s="51" t="s">
-        <v>157</v>
+      <c r="B76" s="16">
+        <v>40.0</v>
       </c>
       <c r="C76" s="51" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E76" s="51">
         <v>8.0</v>
@@ -3756,7 +3708,7 @@
         <v>3.0</v>
       </c>
       <c r="G76" s="51" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -3775,11 +3727,11 @@
       <c r="A77" s="51">
         <v>8.0</v>
       </c>
-      <c r="B77" s="51" t="s">
-        <v>160</v>
+      <c r="B77" s="16">
+        <v>32.0</v>
       </c>
       <c r="C77" s="51" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="E77" s="51">
         <v>9.0</v>
@@ -3788,7 +3740,7 @@
         <v>2.0</v>
       </c>
       <c r="G77" s="51" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
@@ -3808,11 +3760,11 @@
       <c r="A78" s="51">
         <v>8.0</v>
       </c>
-      <c r="B78" s="51" t="s">
-        <v>163</v>
+      <c r="B78" s="16">
+        <v>33.0</v>
       </c>
       <c r="C78" s="51" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="E78" s="51">
         <v>10.0</v>
@@ -3821,11 +3773,11 @@
         <v>2.0</v>
       </c>
       <c r="G78" s="51" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="H78" s="30"/>
-      <c r="I78" s="36" t="s">
-        <v>166</v>
+      <c r="I78" s="62" t="s">
+        <v>145</v>
       </c>
       <c r="M78" s="4"/>
       <c r="N78" s="10"/>
@@ -3842,24 +3794,24 @@
       <c r="A79" s="51">
         <v>9.0</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>22</v>
+      <c r="B79" s="16">
+        <v>16.0</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
-      <c r="I79" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="J79" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K79" s="7" t="s">
-        <v>170</v>
+      <c r="I79" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="J79" s="63" t="s">
+        <v>148</v>
+      </c>
+      <c r="K79" s="63" t="s">
+        <v>149</v>
       </c>
       <c r="M79" s="4"/>
       <c r="N79" s="10"/>
@@ -3876,19 +3828,19 @@
       <c r="A80" s="51">
         <v>9.0</v>
       </c>
-      <c r="B80" s="51" t="s">
-        <v>171</v>
+      <c r="B80" s="16">
+        <v>17.0</v>
       </c>
       <c r="C80" s="51" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="I80" s="16">
         <v>1.0</v>
       </c>
-      <c r="J80" s="58" t="s">
-        <v>173</v>
-      </c>
-      <c r="K80" s="59">
+      <c r="J80" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="K80" s="65">
         <v>0.0</v>
       </c>
       <c r="M80" s="4"/>
@@ -3906,20 +3858,20 @@
       <c r="A81" s="51">
         <v>9.0</v>
       </c>
-      <c r="B81" s="51" t="s">
-        <v>174</v>
+      <c r="B81" s="16">
+        <v>8.0</v>
       </c>
       <c r="C81" s="51" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="I81" s="16">
         <v>2.0</v>
       </c>
-      <c r="J81" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="K81" s="59" t="s">
-        <v>177</v>
+      <c r="J81" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="K81" s="66">
+        <v>7.99</v>
       </c>
       <c r="M81" s="4"/>
       <c r="N81" s="10"/>
@@ -3936,20 +3888,20 @@
       <c r="A82" s="51">
         <v>9.0</v>
       </c>
-      <c r="B82" s="51" t="s">
-        <v>178</v>
+      <c r="B82" s="16">
+        <v>9.0</v>
       </c>
       <c r="C82" s="51" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="I82" s="16">
         <v>3.0</v>
       </c>
-      <c r="J82" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="K82" s="59" t="s">
-        <v>181</v>
+      <c r="J82" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="K82" s="66">
+        <v>5.99</v>
       </c>
       <c r="M82" s="4"/>
       <c r="N82" s="10"/>
@@ -3966,20 +3918,20 @@
       <c r="A83" s="51">
         <v>10.0</v>
       </c>
-      <c r="B83" s="16" t="s">
-        <v>26</v>
+      <c r="B83" s="16">
+        <v>20.0</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="I83" s="16">
         <v>4.0</v>
       </c>
-      <c r="J83" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="K83" s="59" t="s">
-        <v>184</v>
+      <c r="J83" s="64" t="s">
+        <v>157</v>
+      </c>
+      <c r="K83" s="66">
+        <v>6.99</v>
       </c>
       <c r="M83" s="4"/>
       <c r="N83" s="10"/>
@@ -3996,11 +3948,11 @@
       <c r="A84" s="51">
         <v>10.0</v>
       </c>
-      <c r="B84" s="51" t="s">
-        <v>106</v>
+      <c r="B84" s="16">
+        <v>21.0</v>
       </c>
       <c r="C84" s="51" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="M84" s="4"/>
       <c r="N84" s="10"/>
@@ -4017,11 +3969,11 @@
       <c r="A85" s="51">
         <v>10.0</v>
       </c>
-      <c r="B85" s="51" t="s">
-        <v>129</v>
+      <c r="B85" s="16">
+        <v>12.0</v>
       </c>
       <c r="C85" s="51" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="M85" s="4"/>
       <c r="N85" s="10"/>
@@ -4038,11 +3990,11 @@
       <c r="A86" s="51">
         <v>10.0</v>
       </c>
-      <c r="B86" s="51" t="s">
-        <v>187</v>
+      <c r="B86" s="16">
+        <v>13.0</v>
       </c>
       <c r="C86" s="51" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="M86" s="4"/>
       <c r="N86" s="10"/>
@@ -7092,13 +7044,13 @@
   <mergeCells count="10">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A47:C47"/>
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="E67:G67"/>
     <mergeCell ref="J43:K43"/>
     <mergeCell ref="M43:N43"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="H22:K22"/>
+    <mergeCell ref="A47:C47"/>
     <mergeCell ref="I78:K78"/>
   </mergeCells>
   <printOptions/>
@@ -7126,508 +7078,508 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="67">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="C2" s="67">
+        <v>23.0</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="67">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="67">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="67">
+        <v>35.0</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="67">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="67">
+        <v>20.0</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="67">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="67">
+        <v>45.0</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="67">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="67">
+        <v>58.0</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="67" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="67">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="67">
+        <v>33.0</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="67">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="67">
+        <v>26.0</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="68" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="67">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="67">
+        <v>19.0</v>
+      </c>
+      <c r="D9" s="68" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="67">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="67">
+        <v>42.0</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="68" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="67">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="67">
+        <v>46.0</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="67">
+        <v>1.0</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="60" t="s">
+      <c r="F14" s="67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="67">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="68" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="60">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="60">
-        <v>23.0</v>
-      </c>
-      <c r="D2" s="61" t="s">
+      <c r="E15" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="F15" s="67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="67">
+        <v>3.0</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="68" t="s">
         <v>192</v>
       </c>
-      <c r="F2" s="60" t="s">
-        <v>173</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="60">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="60">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="60">
-        <v>35.0</v>
-      </c>
-      <c r="D3" s="61" t="s">
+      <c r="E16" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="F16" s="67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="67">
+        <v>4.0</v>
+      </c>
+      <c r="B17" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="F3" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="H3" s="60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="60">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="60">
-        <v>20.0</v>
-      </c>
-      <c r="D4" s="61" t="s">
+      <c r="E17" s="67" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="F17" s="67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="67">
+        <v>5.0</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="68" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="G4" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="H4" s="60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="60">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="60">
-        <v>45.0</v>
-      </c>
-      <c r="D5" s="61" t="s">
+      <c r="E18" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="F18" s="67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="67">
+        <v>6.0</v>
+      </c>
+      <c r="B19" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="F5" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="G5" s="60" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" s="60" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="60">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="60">
-        <v>58.0</v>
-      </c>
-      <c r="D6" s="61" t="s">
+      <c r="E19" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="F19" s="67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="67">
+        <v>7.0</v>
+      </c>
+      <c r="B20" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="68" t="s">
         <v>200</v>
       </c>
-      <c r="F6" s="60" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" s="60" t="s">
-        <v>151</v>
-      </c>
-      <c r="H6" s="60" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="60">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="60">
-        <v>33.0</v>
-      </c>
-      <c r="D7" s="61" t="s">
+      <c r="E20" s="67" t="s">
         <v>201</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="F20" s="67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="67">
+        <v>8.0</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="F7" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="60" t="s">
-        <v>154</v>
-      </c>
-      <c r="H7" s="60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="60">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="60">
-        <v>26.0</v>
-      </c>
-      <c r="D8" s="61" t="s">
+      <c r="E21" s="67" t="s">
         <v>203</v>
       </c>
-      <c r="E8" s="61" t="s">
+      <c r="F21" s="67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="67">
+        <v>9.0</v>
+      </c>
+      <c r="B22" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="F8" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" s="60" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" s="60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="60">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="60">
-        <v>19.0</v>
-      </c>
-      <c r="D9" s="61" t="s">
+      <c r="E22" s="67" t="s">
         <v>205</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="F22" s="67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="67">
+        <v>10.0</v>
+      </c>
+      <c r="B23" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="68" t="s">
         <v>206</v>
       </c>
-      <c r="F9" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="G9" s="60" t="s">
-        <v>159</v>
-      </c>
-      <c r="H9" s="60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="60">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" s="60">
-        <v>42.0</v>
-      </c>
-      <c r="D10" s="61" t="s">
+      <c r="E23" s="67" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="61" t="s">
-        <v>208</v>
-      </c>
-      <c r="F10" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="H10" s="60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="60">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="60">
-        <v>46.0</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>209</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>210</v>
-      </c>
-      <c r="F11" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="H11" s="60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="60">
-        <v>1.0</v>
-      </c>
-      <c r="B14" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="61" t="s">
-        <v>213</v>
-      </c>
-      <c r="E14" s="60" t="s">
-        <v>214</v>
-      </c>
-      <c r="F14" s="60" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="60">
-        <v>2.0</v>
-      </c>
-      <c r="B15" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="61" t="s">
-        <v>215</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>216</v>
-      </c>
-      <c r="F15" s="60" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="60">
-        <v>3.0</v>
-      </c>
-      <c r="B16" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="61" t="s">
-        <v>217</v>
-      </c>
-      <c r="E16" s="60" t="s">
-        <v>218</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="60">
-        <v>4.0</v>
-      </c>
-      <c r="B17" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>219</v>
-      </c>
-      <c r="E17" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="60">
-        <v>5.0</v>
-      </c>
-      <c r="B18" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="60" t="s">
-        <v>222</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="60">
-        <v>6.0</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="61" t="s">
-        <v>223</v>
-      </c>
-      <c r="E19" s="60" t="s">
-        <v>224</v>
-      </c>
-      <c r="F19" s="60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="60">
-        <v>7.0</v>
-      </c>
-      <c r="B20" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="E20" s="60" t="s">
-        <v>226</v>
-      </c>
-      <c r="F20" s="60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="60">
-        <v>8.0</v>
-      </c>
-      <c r="B21" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="61" t="s">
-        <v>227</v>
-      </c>
-      <c r="E21" s="60" t="s">
-        <v>228</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="60">
-        <v>9.0</v>
-      </c>
-      <c r="B22" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="61" t="s">
-        <v>229</v>
-      </c>
-      <c r="E22" s="60" t="s">
-        <v>230</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="60">
-        <v>10.0</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="61" t="s">
-        <v>231</v>
-      </c>
-      <c r="E23" s="60" t="s">
-        <v>232</v>
-      </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="67" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>